<commit_message>
fixed the formatining in the international
</commit_message>
<xml_diff>
--- a/International Logistics Association Memberships - Data for Cleaning.xlsx
+++ b/International Logistics Association Memberships - Data for Cleaning.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Association ABC memberships" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="351">
   <si>
     <t>Member ID</t>
   </si>
@@ -106,7 +107,7 @@
     <t>Student Associate</t>
   </si>
   <si>
-    <t>CSCP, CLTD</t>
+    <t>CSCP</t>
   </si>
   <si>
     <t>Meneses Contreras</t>
@@ -163,7 +164,7 @@
     <t>L1R 1G1</t>
   </si>
   <si>
-    <t>CSCP, CPIM</t>
+    <t>CPIM</t>
   </si>
   <si>
     <t>Andreu</t>
@@ -205,7 +206,10 @@
     <t>200120 Shanghai</t>
   </si>
   <si>
-    <t>SCOR-P, CLTD, CSCP, PMP</t>
+    <t>SCOR-P</t>
+  </si>
+  <si>
+    <t>PMP</t>
   </si>
   <si>
     <t>He</t>
@@ -304,9 +308,6 @@
     <t>V3J 1P1</t>
   </si>
   <si>
-    <t>PMP, CLTD</t>
-  </si>
-  <si>
     <t>de Alava Casado</t>
   </si>
   <si>
@@ -364,9 +365,6 @@
     <t>New Zealand</t>
   </si>
   <si>
-    <t>CSCP, CPIM, PMP</t>
-  </si>
-  <si>
     <t>Sanseau</t>
   </si>
   <si>
@@ -487,9 +485,6 @@
     <t>446-744</t>
   </si>
   <si>
-    <t>CLTD, PMP</t>
-  </si>
-  <si>
     <t>Venghatachari</t>
   </si>
   <si>
@@ -523,9 +518,6 @@
     <t>Malaysia</t>
   </si>
   <si>
-    <t>SCOR-P, CLTD</t>
-  </si>
-  <si>
     <t>Hagen</t>
   </si>
   <si>
@@ -550,7 +542,7 @@
     <t>100176 China</t>
   </si>
   <si>
-    <t>CPL, CSCP</t>
+    <t>CPL</t>
   </si>
   <si>
     <t>Acheson</t>
@@ -568,9 +560,6 @@
     <t>V1Y 3G9</t>
   </si>
   <si>
-    <t>PMP</t>
-  </si>
-  <si>
     <t>Rojo</t>
   </si>
   <si>
@@ -1073,9 +1062,6 @@
   </si>
   <si>
     <t>H4M 2S9</t>
-  </si>
-  <si>
-    <t>CPIM, CSCP, CLTD</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1186,7 +1172,17 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
     <dxf>
       <font/>
       <fill>
@@ -1227,9 +1223,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle count="3" pivot="0" name="Association ABC memberships-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="2" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -1239,23 +1235,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L75" displayName="Table_1" name="Table_1" id="1">
-  <tableColumns count="12">
-    <tableColumn name="Member ID" id="1"/>
-    <tableColumn name="Last name" id="2"/>
-    <tableColumn name="First name" id="3"/>
-    <tableColumn name="Address 1" id="4"/>
-    <tableColumn name="Address 2" id="5"/>
-    <tableColumn name="Address 3" id="6"/>
-    <tableColumn name="Address 4" id="7"/>
-    <tableColumn name="Address 5" id="8"/>
-    <tableColumn name="Dues amount" id="9"/>
-    <tableColumn name="Membership valid through" id="10"/>
-    <tableColumn name="Member type" id="11"/>
-    <tableColumn name="Certification" id="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:O75" displayName="Table_1" name="Table_1" id="1">
+  <tableColumns count="15">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+    <tableColumn name="Column11" id="11"/>
+    <tableColumn name="Column12" id="12"/>
+    <tableColumn name="Column13" id="13"/>
+    <tableColumn name="Column14" id="14"/>
+    <tableColumn name="Column15" id="15"/>
   </tableColumns>
   <tableStyleInfo name="Association ABC memberships-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
 </table>
 </file>
 
@@ -1322,9 +1330,9 @@
       <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
       <c r="P1" s="7"/>
     </row>
     <row r="2">
@@ -1360,9 +1368,9 @@
       <c r="L2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3">
@@ -1396,9 +1404,9 @@
         <v>24</v>
       </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
       <c r="P3" s="11"/>
     </row>
     <row r="4">
@@ -1436,9 +1444,11 @@
       <c r="L4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="M4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5">
@@ -1474,9 +1484,9 @@
         <v>24</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
       <c r="P5" s="11"/>
     </row>
     <row r="6">
@@ -1512,9 +1522,9 @@
         <v>17</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6" s="11"/>
     </row>
     <row r="7">
@@ -1552,11 +1562,13 @@
         <v>30</v>
       </c>
       <c r="L7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8">
@@ -1590,9 +1602,9 @@
         <v>17</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="11"/>
     </row>
     <row r="9">
@@ -1626,9 +1638,9 @@
         <v>17</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
       <c r="P9" s="11"/>
     </row>
     <row r="10">
@@ -1664,9 +1676,15 @@
       <c r="L10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="M10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="P10" s="7"/>
     </row>
     <row r="11">
@@ -1674,16 +1692,16 @@
         <v>100020.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>47</v>
@@ -1692,7 +1710,7 @@
         <v>48</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I11" s="8">
         <v>200.0</v>
@@ -1704,9 +1722,9 @@
         <v>17</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="11"/>
     </row>
     <row r="12">
@@ -1714,16 +1732,16 @@
         <v>100021.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="4" t="s">
@@ -1742,9 +1760,9 @@
         <v>17</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="11"/>
     </row>
     <row r="13">
@@ -1752,20 +1770,20 @@
         <v>100022.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="12">
@@ -1778,9 +1796,9 @@
         <v>30</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
       <c r="P13" s="11"/>
     </row>
     <row r="14">
@@ -1788,20 +1806,20 @@
         <v>100023.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="12">
@@ -1816,9 +1834,9 @@
       <c r="L14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
       <c r="P14" s="7"/>
     </row>
     <row r="15">
@@ -1826,16 +1844,16 @@
         <v>100024.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4" t="s">
@@ -1852,9 +1870,9 @@
         <v>30</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="11"/>
     </row>
     <row r="16">
@@ -1862,16 +1880,16 @@
         <v>100025.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>42</v>
@@ -1890,9 +1908,9 @@
         <v>17</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="11"/>
     </row>
     <row r="17">
@@ -1900,25 +1918,25 @@
         <v>100026.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I17" s="8">
         <v>200.0</v>
@@ -1930,11 +1948,13 @@
         <v>17</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
       <c r="P17" s="7"/>
     </row>
     <row r="18">
@@ -1970,9 +1990,9 @@
         <v>24</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
       <c r="P18" s="11"/>
     </row>
     <row r="19">
@@ -2010,9 +2030,9 @@
         <v>17</v>
       </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
       <c r="P19" s="11"/>
     </row>
     <row r="20">
@@ -2046,9 +2066,9 @@
         <v>17</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
       <c r="P20" s="11"/>
     </row>
     <row r="21">
@@ -2084,11 +2104,15 @@
         <v>30</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O21" s="6"/>
       <c r="P21" s="7"/>
     </row>
     <row r="22">
@@ -2096,20 +2120,20 @@
         <v>100031.0</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="8">
@@ -2122,9 +2146,9 @@
         <v>30</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
       <c r="P22" s="11"/>
     </row>
     <row r="23">
@@ -2132,16 +2156,16 @@
         <v>100032.0</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>126</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>47</v>
@@ -2150,7 +2174,7 @@
         <v>48</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I23" s="8">
         <v>100.0</v>
@@ -2162,9 +2186,9 @@
         <v>30</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
       <c r="P23" s="11"/>
     </row>
     <row r="24">
@@ -2172,16 +2196,16 @@
         <v>100033.0</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="4" t="s">
@@ -2200,9 +2224,9 @@
         <v>17</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
       <c r="P24" s="11"/>
     </row>
     <row r="25">
@@ -2210,23 +2234,23 @@
         <v>100034.0</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="I25" s="8">
         <v>200.0</v>
@@ -2238,9 +2262,9 @@
         <v>17</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
       <c r="P25" s="11"/>
     </row>
     <row r="26">
@@ -2248,25 +2272,25 @@
         <v>100035.0</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I26" s="8">
         <v>200.0</v>
@@ -2278,9 +2302,9 @@
         <v>17</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
       <c r="P26" s="11"/>
     </row>
     <row r="27">
@@ -2288,20 +2312,20 @@
         <v>100036.0</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="8">
@@ -2314,11 +2338,13 @@
         <v>30</v>
       </c>
       <c r="L27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
       <c r="P27" s="7"/>
     </row>
     <row r="28">
@@ -2326,16 +2352,16 @@
         <v>100037.0</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>47</v>
@@ -2344,7 +2370,7 @@
         <v>48</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I28" s="8">
         <v>200.0</v>
@@ -2356,29 +2382,32 @@
         <v>17</v>
       </c>
       <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
     </row>
     <row r="29">
       <c r="A29" s="1">
         <v>100038.0</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="I29" s="8">
         <v>200.0</v>
@@ -2390,11 +2419,13 @@
         <v>17</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="7"/>
     </row>
     <row r="30">
@@ -2402,19 +2433,19 @@
         <v>100039.0</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="E30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>59</v>
@@ -2432,28 +2463,31 @@
         <v>17</v>
       </c>
       <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
     </row>
     <row r="31">
       <c r="A31" s="1">
         <v>100040.0</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="8">
@@ -2466,11 +2500,13 @@
         <v>17</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
       <c r="P31" s="7"/>
     </row>
     <row r="32">
@@ -2478,20 +2514,20 @@
         <v>100041.0</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="8">
@@ -2504,22 +2540,25 @@
         <v>30</v>
       </c>
       <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
     </row>
     <row r="33">
       <c r="A33" s="1">
         <v>100042.0</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="4" t="s">
@@ -2536,11 +2575,13 @@
         <v>17</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="M33" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
       <c r="P33" s="11"/>
     </row>
     <row r="34">
@@ -2548,25 +2589,25 @@
         <v>100043.0</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I34" s="8">
         <v>200.0</v>
@@ -2578,11 +2619,11 @@
         <v>17</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
       <c r="P34" s="7"/>
     </row>
     <row r="35">
@@ -2590,20 +2631,20 @@
         <v>1000444.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="8">
@@ -2616,9 +2657,9 @@
         <v>17</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
       <c r="P35" s="17"/>
     </row>
     <row r="36">
@@ -2626,20 +2667,20 @@
         <v>100045.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H36" s="3">
         <v>10120.0</v>
@@ -2654,11 +2695,13 @@
         <v>17</v>
       </c>
       <c r="L36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
       <c r="P36" s="7"/>
     </row>
     <row r="37">
@@ -2666,16 +2709,16 @@
         <v>100046.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>47</v>
@@ -2684,7 +2727,7 @@
         <v>48</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I37" s="8">
         <v>200.0</v>
@@ -2696,9 +2739,9 @@
         <v>17</v>
       </c>
       <c r="L37" s="4"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
       <c r="P37" s="11"/>
     </row>
     <row r="38">
@@ -2706,20 +2749,20 @@
         <v>100047.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="8">
@@ -2732,11 +2775,11 @@
         <v>17</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
+        <v>201</v>
+      </c>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
       <c r="P38" s="7"/>
     </row>
     <row r="39">
@@ -2744,16 +2787,16 @@
         <v>100048.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>36</v>
@@ -2774,9 +2817,9 @@
         <v>17</v>
       </c>
       <c r="L39" s="4"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
       <c r="P39" s="11"/>
     </row>
     <row r="40">
@@ -2784,20 +2827,20 @@
         <v>100049.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="8">
@@ -2810,11 +2853,11 @@
         <v>30</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
+        <v>211</v>
+      </c>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
       <c r="P40" s="7"/>
     </row>
     <row r="41">
@@ -2822,23 +2865,23 @@
         <v>100050.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I41" s="8">
         <v>100.0</v>
@@ -2850,9 +2893,9 @@
         <v>30</v>
       </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
       <c r="P41" s="11"/>
     </row>
     <row r="42">
@@ -2860,23 +2903,23 @@
         <v>100051.0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I42" s="8">
         <v>200.0</v>
@@ -2888,9 +2931,9 @@
         <v>17</v>
       </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
       <c r="P42" s="7"/>
     </row>
     <row r="43">
@@ -2898,16 +2941,16 @@
         <v>100053.0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="4" t="s">
@@ -2924,9 +2967,9 @@
         <v>30</v>
       </c>
       <c r="L43" s="4"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
       <c r="P43" s="11"/>
     </row>
     <row r="44">
@@ -2934,16 +2977,16 @@
         <v>100054.0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="4" t="s">
@@ -2962,11 +3005,11 @@
         <v>24</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
+        <v>231</v>
+      </c>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
       <c r="P44" s="11"/>
     </row>
     <row r="45">
@@ -2974,16 +3017,16 @@
         <v>100055.0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="4" t="s">
@@ -3002,9 +3045,9 @@
         <v>24</v>
       </c>
       <c r="L45" s="4"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
       <c r="P45" s="11"/>
     </row>
     <row r="46">
@@ -3012,16 +3055,16 @@
         <v>100056.0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="4" t="s">
@@ -3038,9 +3081,9 @@
         <v>17</v>
       </c>
       <c r="L46" s="4"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
       <c r="P46" s="7"/>
     </row>
     <row r="47">
@@ -3048,16 +3091,16 @@
         <v>100057.0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>47</v>
@@ -3066,7 +3109,7 @@
         <v>48</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I47" s="8">
         <v>200.0</v>
@@ -3078,9 +3121,9 @@
         <v>17</v>
       </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
       <c r="P47" s="11"/>
     </row>
     <row r="48">
@@ -3088,16 +3131,16 @@
         <v>100058.0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>47</v>
@@ -3106,7 +3149,7 @@
         <v>48</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I48" s="8">
         <v>500.0</v>
@@ -3118,11 +3161,11 @@
         <v>24</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
+        <v>248</v>
+      </c>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
       <c r="P48" s="11"/>
     </row>
     <row r="49">
@@ -3130,16 +3173,16 @@
         <v>100059.0</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>47</v>
@@ -3148,7 +3191,7 @@
         <v>48</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I49" s="8">
         <v>200.0</v>
@@ -3160,9 +3203,9 @@
         <v>17</v>
       </c>
       <c r="L49" s="4"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
       <c r="P49" s="11"/>
     </row>
     <row r="50">
@@ -3170,20 +3213,20 @@
         <v>100060.0</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="8">
@@ -3196,9 +3239,9 @@
         <v>17</v>
       </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
       <c r="P50" s="7"/>
     </row>
     <row r="51">
@@ -3206,20 +3249,20 @@
         <v>100061.0</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="8">
@@ -3232,11 +3275,13 @@
         <v>24</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
       <c r="P51" s="11"/>
     </row>
     <row r="52">
@@ -3244,16 +3289,16 @@
         <v>100063.0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>47</v>
@@ -3262,7 +3307,7 @@
         <v>48</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I52" s="8">
         <v>200.0</v>
@@ -3274,9 +3319,9 @@
         <v>17</v>
       </c>
       <c r="L52" s="4"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
       <c r="P52" s="11"/>
     </row>
     <row r="53">
@@ -3284,16 +3329,16 @@
         <v>100064.0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>47</v>
@@ -3302,7 +3347,7 @@
         <v>48</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I53" s="8">
         <v>200.0</v>
@@ -3314,9 +3359,9 @@
         <v>17</v>
       </c>
       <c r="L53" s="4"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
       <c r="P53" s="7"/>
     </row>
     <row r="54">
@@ -3324,25 +3369,25 @@
         <v>100065.0</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I54" s="12">
         <v>-200.0</v>
@@ -3354,9 +3399,9 @@
         <v>17</v>
       </c>
       <c r="L54" s="4"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
       <c r="P54" s="11"/>
     </row>
     <row r="55">
@@ -3364,23 +3409,23 @@
         <v>100066.0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I55" s="8">
         <v>200.0</v>
@@ -3392,9 +3437,9 @@
         <v>17</v>
       </c>
       <c r="L55" s="4"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
       <c r="P55" s="11"/>
     </row>
     <row r="56">
@@ -3402,16 +3447,16 @@
         <v>100067.0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>47</v>
@@ -3420,7 +3465,7 @@
         <v>48</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I56" s="8">
         <v>200.0</v>
@@ -3432,9 +3477,9 @@
         <v>17</v>
       </c>
       <c r="L56" s="4"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
       <c r="P56" s="11"/>
     </row>
     <row r="57">
@@ -3442,16 +3487,16 @@
         <v>100068.0</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>47</v>
@@ -3460,7 +3505,7 @@
         <v>48</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I57" s="8">
         <v>500.0</v>
@@ -3472,11 +3517,11 @@
         <v>24</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
+        <v>295</v>
+      </c>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
       <c r="P57" s="11"/>
     </row>
     <row r="58">
@@ -3484,25 +3529,25 @@
         <v>100069.0</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>304</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I58" s="8">
         <v>500.0</v>
@@ -3514,9 +3559,9 @@
         <v>24</v>
       </c>
       <c r="L58" s="4"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
       <c r="P58" s="11"/>
     </row>
     <row r="59">
@@ -3524,25 +3569,25 @@
         <v>100070.0</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I59" s="8">
         <v>200.0</v>
@@ -3551,12 +3596,12 @@
         <v>44268.0</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="L59" s="4"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
       <c r="P59" s="7"/>
     </row>
     <row r="60">
@@ -3564,18 +3609,18 @@
         <v>100071.0</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="8">
@@ -3588,9 +3633,9 @@
         <v>30</v>
       </c>
       <c r="L60" s="4"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
       <c r="P60" s="11"/>
     </row>
     <row r="61">
@@ -3598,18 +3643,18 @@
         <v>100072.0</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="8">
@@ -3622,9 +3667,9 @@
         <v>30</v>
       </c>
       <c r="L61" s="4"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
       <c r="P61" s="11"/>
     </row>
     <row r="62">
@@ -3632,20 +3677,20 @@
         <v>100073.0</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H62" s="10"/>
       <c r="I62" s="8">
@@ -3660,9 +3705,9 @@
       <c r="L62" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
-      <c r="O62" s="11"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
       <c r="P62" s="11"/>
     </row>
     <row r="63">
@@ -3670,16 +3715,16 @@
         <v>100074.0</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>47</v>
@@ -3688,7 +3733,7 @@
         <v>48</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I63" s="8">
         <v>200.0</v>
@@ -3700,9 +3745,9 @@
         <v>17</v>
       </c>
       <c r="L63" s="4"/>
-      <c r="M63" s="11"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
       <c r="P63" s="11"/>
     </row>
     <row r="64">
@@ -3710,20 +3755,20 @@
         <v>100075.0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="8">
@@ -3736,9 +3781,9 @@
         <v>30</v>
       </c>
       <c r="L64" s="4"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
       <c r="P64" s="7"/>
     </row>
     <row r="65">
@@ -3746,16 +3791,16 @@
         <v>100076.0</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>47</v>
@@ -3764,7 +3809,7 @@
         <v>48</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I65" s="8">
         <v>200.0</v>
@@ -3776,9 +3821,9 @@
         <v>17</v>
       </c>
       <c r="L65" s="4"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
       <c r="P65" s="11"/>
     </row>
     <row r="66">
@@ -3786,19 +3831,19 @@
         <v>100077.0</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>336</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>37</v>
@@ -3814,11 +3859,11 @@
         <v>17</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
+        <v>295</v>
+      </c>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
       <c r="P66" s="11"/>
     </row>
     <row r="67">
@@ -3826,20 +3871,20 @@
         <v>100078.0</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="8"/>
@@ -3850,9 +3895,9 @@
         <v>30</v>
       </c>
       <c r="L67" s="4"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
       <c r="P67" s="11"/>
     </row>
     <row r="68">
@@ -3860,20 +3905,20 @@
         <v>100079.0</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="8">
@@ -3886,11 +3931,11 @@
         <v>30</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="M68" s="7"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
+        <v>248</v>
+      </c>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
       <c r="P68" s="7"/>
     </row>
     <row r="69">
@@ -3898,25 +3943,25 @@
         <v>100080.0</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I69" s="8">
         <v>200.0</v>
@@ -3928,9 +3973,9 @@
         <v>17</v>
       </c>
       <c r="L69" s="4"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
       <c r="P69" s="11"/>
     </row>
     <row r="70">
@@ -3938,25 +3983,25 @@
         <v>100081.0</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="I70" s="8">
         <v>500.0</v>
@@ -3968,11 +4013,15 @@
         <v>24</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O70" s="6"/>
       <c r="P70" s="7"/>
     </row>
     <row r="71">
@@ -3980,16 +4029,16 @@
         <v>100082.0</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="4" t="s">
@@ -4006,16 +4055,13 @@
         <v>17</v>
       </c>
       <c r="L71" s="4"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
       <c r="P71" s="11"/>
     </row>
     <row r="72">
       <c r="J72" s="19"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
       <c r="P72" s="7"/>
     </row>
     <row r="73">
@@ -4031,9 +4077,9 @@
       <c r="J73" s="20"/>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
       <c r="P73" s="11"/>
     </row>
     <row r="74">
@@ -4046,14 +4092,14 @@
       <c r="G74" s="4"/>
       <c r="H74" s="11"/>
       <c r="I74" s="6" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J74" s="20"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
       <c r="P74" s="11"/>
     </row>
     <row r="75">
@@ -4066,20 +4112,39 @@
       <c r="G75" s="4"/>
       <c r="H75" s="11"/>
       <c r="I75" s="6" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J75" s="20"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="11"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
       <c r="P75" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:E75 I1:P75 G1:G75">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>